<commit_message>
[Modified] : File Export_Print Specification.xlsx
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Document/Diagram/UseCase/Export_Print/Export_Print Specification.xlsx
+++ b/ToDoApp-Doc/Document/Diagram/UseCase/Export_Print/Export_Print Specification.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Netpham1970\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Netpham1970\Desktop\pullcc\To-Do-App\ToDoApp-Doc\Document\Diagram\UseCase\Export_Print\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C6BA2C-407A-4673-AD48-9E0E05BFE876}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCC2714-ED09-46D4-836A-F79E15420EBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -606,23 +606,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -639,9 +627,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -650,6 +635,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -886,120 +886,120 @@
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="2:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="14"/>
     </row>
     <row r="7" spans="2:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="16"/>
+      <c r="C9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="14"/>
     </row>
     <row r="11" spans="2:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="14"/>
     </row>
     <row r="12" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="14"/>
     </row>
     <row r="13" spans="2:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="14"/>
     </row>
     <row r="14" spans="2:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="14"/>
     </row>
     <row r="15" spans="2:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="4"/>
+      <c r="D15" s="14"/>
     </row>
     <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2005,139 +2005,139 @@
   <dimension ref="B3:D1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="29.375" style="10" customWidth="1"/>
-    <col min="3" max="3" width="22.25" style="10" customWidth="1"/>
-    <col min="4" max="4" width="23.25" style="10" customWidth="1"/>
-    <col min="5" max="26" width="7.625" style="10" customWidth="1"/>
-    <col min="27" max="16384" width="12.625" style="10"/>
+    <col min="1" max="1" width="7.625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="29.375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="22.25" style="6" customWidth="1"/>
+    <col min="4" max="4" width="23.25" style="6" customWidth="1"/>
+    <col min="5" max="26" width="7.625" style="6" customWidth="1"/>
+    <col min="27" max="16384" width="12.625" style="6"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="2:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="14"/>
     </row>
     <row r="7" spans="2:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
-      <c r="C9" s="17" t="s">
+      <c r="B9" s="16"/>
+      <c r="C9" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="12" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="14"/>
     </row>
     <row r="11" spans="2:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="14"/>
     </row>
     <row r="12" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="14"/>
     </row>
     <row r="13" spans="2:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="14"/>
     </row>
     <row r="14" spans="2:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="14"/>
     </row>
     <row r="15" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="4"/>
+      <c r="D15" s="14"/>
     </row>
     <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3148,143 +3148,143 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="31.25" style="10" customWidth="1"/>
-    <col min="3" max="3" width="18.625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="35.5" style="10" customWidth="1"/>
-    <col min="5" max="26" width="7.625" style="10" customWidth="1"/>
-    <col min="27" max="16384" width="12.625" style="10"/>
+    <col min="1" max="1" width="7.625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="31.25" style="6" customWidth="1"/>
+    <col min="3" max="3" width="18.625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="35.5" style="6" customWidth="1"/>
+    <col min="5" max="26" width="7.625" style="6" customWidth="1"/>
+    <col min="27" max="16384" width="12.625" style="6"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="2:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="14"/>
     </row>
     <row r="7" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="14"/>
-      <c r="C9" s="13" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="15" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="14"/>
     </row>
     <row r="12" spans="2:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="14"/>
     </row>
     <row r="13" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="14"/>
     </row>
     <row r="14" spans="2:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="14"/>
     </row>
     <row r="15" spans="2:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="4"/>
+      <c r="D15" s="14"/>
     </row>
     <row r="16" spans="2:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="4"/>
+      <c r="D16" s="14"/>
     </row>
     <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4295,143 +4295,143 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="31.125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="25.375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="31.375" style="10" customWidth="1"/>
-    <col min="5" max="26" width="7.625" style="10" customWidth="1"/>
-    <col min="27" max="16384" width="12.625" style="10"/>
+    <col min="1" max="1" width="7.625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="31.125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="25.375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="31.375" style="6" customWidth="1"/>
+    <col min="5" max="26" width="7.625" style="6" customWidth="1"/>
+    <col min="27" max="16384" width="12.625" style="6"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="2:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="14"/>
     </row>
     <row r="7" spans="2:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="14"/>
-      <c r="C9" s="16" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="15" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="14"/>
     </row>
     <row r="12" spans="2:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="14"/>
     </row>
     <row r="13" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="14"/>
     </row>
     <row r="14" spans="2:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="14"/>
     </row>
     <row r="15" spans="2:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="4"/>
+      <c r="D15" s="14"/>
     </row>
     <row r="16" spans="2:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="4"/>
+      <c r="D16" s="14"/>
     </row>
     <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5442,143 +5442,143 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="29.875" style="10" customWidth="1"/>
-    <col min="3" max="3" width="22.75" style="10" customWidth="1"/>
-    <col min="4" max="4" width="37.875" style="10" customWidth="1"/>
-    <col min="5" max="26" width="7.625" style="10" customWidth="1"/>
-    <col min="27" max="16384" width="12.625" style="10"/>
+    <col min="1" max="1" width="7.625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="29.875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="22.75" style="6" customWidth="1"/>
+    <col min="4" max="4" width="37.875" style="6" customWidth="1"/>
+    <col min="5" max="26" width="7.625" style="6" customWidth="1"/>
+    <col min="27" max="16384" width="12.625" style="6"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="2:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="14"/>
     </row>
     <row r="7" spans="2:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="14"/>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="17" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="12" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="14"/>
     </row>
     <row r="12" spans="2:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="14"/>
     </row>
     <row r="13" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="14"/>
     </row>
     <row r="14" spans="2:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="14"/>
     </row>
     <row r="15" spans="2:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="4"/>
+      <c r="D15" s="14"/>
     </row>
     <row r="16" spans="2:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="4"/>
+      <c r="D16" s="14"/>
     </row>
     <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6589,143 +6589,143 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="31" style="10" customWidth="1"/>
-    <col min="3" max="3" width="24" style="10" customWidth="1"/>
-    <col min="4" max="4" width="34.625" style="10" customWidth="1"/>
-    <col min="5" max="26" width="7.625" style="10" customWidth="1"/>
-    <col min="27" max="16384" width="12.625" style="10"/>
+    <col min="1" max="1" width="7.625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="31" style="6" customWidth="1"/>
+    <col min="3" max="3" width="24" style="6" customWidth="1"/>
+    <col min="4" max="4" width="34.625" style="6" customWidth="1"/>
+    <col min="5" max="26" width="7.625" style="6" customWidth="1"/>
+    <col min="27" max="16384" width="12.625" style="6"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="2:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="14"/>
     </row>
     <row r="7" spans="2:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="14"/>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="17" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="12" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="14"/>
     </row>
     <row r="12" spans="2:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="14"/>
     </row>
     <row r="13" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="14"/>
     </row>
     <row r="14" spans="2:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="14"/>
     </row>
     <row r="15" spans="2:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="4"/>
+      <c r="D15" s="14"/>
     </row>
     <row r="16" spans="2:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="4"/>
+      <c r="D16" s="14"/>
     </row>
     <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7736,143 +7736,143 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="30.125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="24.625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="35.625" style="10" customWidth="1"/>
-    <col min="5" max="26" width="7.625" style="10" customWidth="1"/>
-    <col min="27" max="16384" width="12.625" style="10"/>
+    <col min="1" max="1" width="7.625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="30.125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="24.625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="35.625" style="6" customWidth="1"/>
+    <col min="5" max="26" width="7.625" style="6" customWidth="1"/>
+    <col min="27" max="16384" width="12.625" style="6"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="2:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="14"/>
     </row>
     <row r="7" spans="2:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="14"/>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="17" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="12" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="14"/>
     </row>
     <row r="12" spans="2:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="14"/>
     </row>
     <row r="13" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="14"/>
     </row>
     <row r="14" spans="2:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="14"/>
     </row>
     <row r="15" spans="2:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="4"/>
+      <c r="D15" s="14"/>
     </row>
     <row r="16" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="4"/>
+      <c r="D16" s="14"/>
     </row>
     <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8861,12 +8861,12 @@
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C12:D12"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -8883,152 +8883,152 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="29.75" style="10" customWidth="1"/>
-    <col min="3" max="3" width="27" style="10" customWidth="1"/>
-    <col min="4" max="4" width="29.75" style="10" customWidth="1"/>
-    <col min="5" max="26" width="7.625" style="10" customWidth="1"/>
-    <col min="27" max="16384" width="12.625" style="10"/>
+    <col min="1" max="1" width="7.625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="29.75" style="6" customWidth="1"/>
+    <col min="3" max="3" width="27" style="6" customWidth="1"/>
+    <col min="4" max="4" width="29.75" style="6" customWidth="1"/>
+    <col min="5" max="26" width="7.625" style="6" customWidth="1"/>
+    <col min="27" max="16384" width="12.625" style="6"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="2:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="14"/>
     </row>
     <row r="7" spans="2:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="14"/>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="14"/>
-      <c r="C10" s="17" t="s">
+      <c r="B10" s="17"/>
+      <c r="C10" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="12" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
-      <c r="C11" s="17" t="s">
+      <c r="B11" s="16"/>
+      <c r="C11" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="12" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="14"/>
     </row>
     <row r="13" spans="2:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="14"/>
     </row>
     <row r="14" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="14"/>
     </row>
     <row r="15" spans="2:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="4"/>
+      <c r="D15" s="14"/>
     </row>
     <row r="16" spans="2:4" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="D16" s="4"/>
+      <c r="D16" s="14"/>
     </row>
     <row r="17" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="4"/>
+      <c r="D17" s="14"/>
     </row>
     <row r="24" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10017,12 +10017,12 @@
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C13:D13"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -10039,123 +10039,123 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="28.375" style="10" customWidth="1"/>
-    <col min="3" max="3" width="23" style="10" customWidth="1"/>
-    <col min="4" max="4" width="27.125" style="10" customWidth="1"/>
-    <col min="5" max="26" width="7.625" style="10" customWidth="1"/>
-    <col min="27" max="16384" width="12.625" style="10"/>
+    <col min="1" max="1" width="7.625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="28.375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="23" style="6" customWidth="1"/>
+    <col min="4" max="4" width="27.125" style="6" customWidth="1"/>
+    <col min="5" max="26" width="7.625" style="6" customWidth="1"/>
+    <col min="27" max="16384" width="12.625" style="6"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="2:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="14"/>
     </row>
     <row r="7" spans="2:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="14"/>
     </row>
     <row r="10" spans="2:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="14"/>
     </row>
     <row r="11" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="14"/>
     </row>
     <row r="12" spans="2:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="14"/>
     </row>
     <row r="13" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="14"/>
     </row>
     <row r="14" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="14"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11165,134 +11165,134 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="28.125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="20" style="10" customWidth="1"/>
-    <col min="4" max="4" width="28.75" style="10" customWidth="1"/>
-    <col min="5" max="26" width="7.625" style="10" customWidth="1"/>
-    <col min="27" max="16384" width="12.625" style="10"/>
+    <col min="1" max="1" width="7.625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="28.125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="20" style="6" customWidth="1"/>
+    <col min="4" max="4" width="28.75" style="6" customWidth="1"/>
+    <col min="5" max="26" width="7.625" style="6" customWidth="1"/>
+    <col min="27" max="16384" width="12.625" style="6"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="2:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="14"/>
     </row>
     <row r="7" spans="2:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
-      <c r="C9" s="17" t="s">
+      <c r="B9" s="16"/>
+      <c r="C9" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="12" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="14"/>
     </row>
     <row r="11" spans="2:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="14"/>
     </row>
     <row r="12" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="14"/>
     </row>
     <row r="13" spans="2:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="14"/>
     </row>
     <row r="14" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="14"/>
     </row>
     <row r="15" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="4"/>
+      <c r="D15" s="14"/>
     </row>
     <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>